<commit_message>
feat: change teh layout of bubble chart for muslim countries
</commit_message>
<xml_diff>
--- a/wit/web_region_bar_MENA/travel_market_summary.xlsx
+++ b/wit/web_region_bar_MENA/travel_market_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/130fda80f0432a83/TravelMarketViz/wit/web_region_bubble_MENA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/130fda80f0432a83/TravelMarketViz/wit/web_region_bar_MENA/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="8" documentId="11_4566CFE2356CD672DB3B3595395BDA16D654840E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8DA88C5-2ED8-A146-8150-041499759ECD}"/>
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F921"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A876" zoomScale="134" workbookViewId="0">
-      <selection activeCell="A883" sqref="A883:F921"/>
+    <sheetView tabSelected="1" topLeftCell="A901" zoomScale="134" workbookViewId="0">
+      <selection activeCell="B915" sqref="B915:B919"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19021,6 +19021,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>